<commit_message>
2020/11/11 operation speed comparison
</commit_message>
<xml_diff>
--- a/operation speed comparison.xlsx
+++ b/operation speed comparison.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\umc19\source\repos\BigIntegerGroup\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\source\repos\BigIntegerGroup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E61E5CAB-F127-4B55-B00D-28AF808C11DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E6683E5-9742-4A07-88C9-513E0684F78D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1980" yWindow="6510" windowWidth="25065" windowHeight="11415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,15 +20,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -44,18 +35,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>8 byte</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>32 byte</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>64 byte</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>sub</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -100,7 +79,19 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>조건: [모든 수는 non_negative, word length = 10], [각 셀은 1000회 연산의 평균값], [mod_exp 연산에서 n = 65537] [div, mod_exp 연산시 flag = 3]</t>
+    <t>8 bit</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>32 bit</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>64 bit</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>조건: [모든 수는 non_negative, bit = 1024], [각 셀의 값은 (그 연산을 1000회 실행하는 시간의 평균값) * 10000], [mod_exp 연산에서 n = 65537] [div, mod_exp 연산시 flag = 4]</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -460,57 +451,57 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S26"/>
+  <dimension ref="A1:S32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="V20" sqref="V20"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="S31" sqref="S31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="9.59765625" customWidth="1"/>
-    <col min="3" max="5" width="14.09765625" customWidth="1"/>
-    <col min="8" max="9" width="9.59765625" customWidth="1"/>
-    <col min="10" max="12" width="14.09765625" customWidth="1"/>
-    <col min="15" max="16" width="9.59765625" customWidth="1"/>
-    <col min="17" max="19" width="14.09765625" customWidth="1"/>
+    <col min="1" max="2" width="9.625" customWidth="1"/>
+    <col min="3" max="5" width="14.125" customWidth="1"/>
+    <col min="8" max="9" width="9.625" customWidth="1"/>
+    <col min="10" max="12" width="14.125" customWidth="1"/>
+    <col min="15" max="16" width="9.625" customWidth="1"/>
+    <col min="17" max="19" width="14.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="C2" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="E2" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="J2" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="K2" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="L2" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="Q2" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="R2" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="S2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -518,1007 +509,1012 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>3.0000000000000001E-6</v>
+        <v>0.19</v>
       </c>
       <c r="D3">
-        <v>6.9999999999999999E-6</v>
+        <v>0.19</v>
       </c>
       <c r="E3">
-        <v>1.2999999999999999E-5</v>
+        <v>0.18</v>
       </c>
       <c r="H3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3">
-        <v>3.0000000000000001E-6</v>
+        <v>0.19</v>
       </c>
       <c r="K3">
-        <v>6.9999999999999999E-6</v>
+        <v>0.18</v>
       </c>
       <c r="L3">
-        <v>1.2E-5</v>
+        <v>0.18</v>
       </c>
       <c r="O3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="P3">
         <v>1</v>
       </c>
       <c r="Q3">
-        <v>2.1999999999999999E-5</v>
+        <v>2.39</v>
       </c>
       <c r="R3">
-        <v>2.8E-5</v>
+        <v>0.72</v>
       </c>
       <c r="S3">
-        <v>3.1999999999999999E-5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.4">
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>2</v>
       </c>
       <c r="C4">
-        <v>3.9999999999999998E-6</v>
+        <v>0.19</v>
       </c>
       <c r="D4">
-        <v>6.9999999999999999E-6</v>
+        <v>0.18</v>
       </c>
       <c r="E4">
-        <v>1.2999999999999999E-5</v>
+        <v>0.18</v>
       </c>
       <c r="I4">
         <v>2</v>
       </c>
       <c r="J4">
-        <v>3.9999999999999998E-6</v>
+        <v>0.19</v>
       </c>
       <c r="K4">
-        <v>6.9999999999999999E-6</v>
+        <v>0.17</v>
       </c>
       <c r="L4">
-        <v>1.2E-5</v>
+        <v>0.17</v>
       </c>
       <c r="P4">
         <v>2</v>
       </c>
       <c r="Q4">
-        <v>2.3E-5</v>
+        <v>2.4</v>
       </c>
       <c r="R4">
-        <v>2.9E-5</v>
+        <v>0.74999999999999989</v>
       </c>
       <c r="S4">
-        <v>3.1999999999999999E-5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.4">
+        <v>0.46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>3</v>
       </c>
       <c r="C5">
-        <v>3.9999999999999998E-6</v>
+        <v>0.19</v>
       </c>
       <c r="D5">
-        <v>6.9999999999999999E-6</v>
+        <v>0.19</v>
       </c>
       <c r="E5">
-        <v>1.2999999999999999E-5</v>
+        <v>0.18</v>
       </c>
       <c r="I5">
         <v>3</v>
       </c>
       <c r="J5">
-        <v>3.9999999999999998E-6</v>
+        <v>0.2</v>
       </c>
       <c r="K5">
-        <v>6.9999999999999999E-6</v>
+        <v>0.18</v>
       </c>
       <c r="L5">
-        <v>1.2E-5</v>
+        <v>0.18</v>
       </c>
       <c r="P5">
         <v>3</v>
       </c>
       <c r="Q5">
-        <v>2.1999999999999999E-5</v>
+        <v>2.3699999999999997</v>
       </c>
       <c r="R5">
-        <v>2.9E-5</v>
+        <v>0.72</v>
       </c>
       <c r="S5">
-        <v>3.1999999999999999E-5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.4">
+        <v>0.46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>4</v>
       </c>
       <c r="C6">
-        <v>3.0000000000000001E-6</v>
+        <v>0.19</v>
       </c>
       <c r="D6">
-        <v>6.9999999999999999E-6</v>
+        <v>0.19</v>
       </c>
       <c r="E6">
-        <v>1.2999999999999999E-5</v>
+        <v>0.18</v>
       </c>
       <c r="I6">
         <v>4</v>
       </c>
       <c r="J6">
-        <v>3.0000000000000001E-6</v>
+        <v>0.22</v>
       </c>
       <c r="K6">
-        <v>6.9999999999999999E-6</v>
+        <v>0.18</v>
       </c>
       <c r="L6">
-        <v>1.2E-5</v>
+        <v>0.17</v>
       </c>
       <c r="P6">
         <v>4</v>
       </c>
       <c r="Q6">
-        <v>2.4000000000000001E-5</v>
+        <v>2.5300000000000002</v>
       </c>
       <c r="R6">
-        <v>2.6999999999999999E-5</v>
+        <v>0.72</v>
       </c>
       <c r="S6">
-        <v>3.1999999999999999E-5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.4">
+        <v>0.46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>5</v>
       </c>
       <c r="C7">
-        <v>3.0000000000000001E-6</v>
+        <v>0.19</v>
       </c>
       <c r="D7">
-        <v>6.9999999999999999E-6</v>
+        <v>0.18</v>
       </c>
       <c r="E7">
-        <v>1.2E-5</v>
+        <v>0.18</v>
       </c>
       <c r="I7">
         <v>5</v>
       </c>
       <c r="J7">
-        <v>3.9999999999999998E-6</v>
+        <v>0.22</v>
       </c>
       <c r="K7">
-        <v>6.9999999999999999E-6</v>
+        <v>0.2</v>
       </c>
       <c r="L7">
-        <v>1.2E-5</v>
+        <v>0.18</v>
       </c>
       <c r="P7">
         <v>5</v>
       </c>
       <c r="Q7">
-        <v>2.1999999999999999E-5</v>
+        <v>2.7399999999999998</v>
       </c>
       <c r="R7">
-        <v>2.5999999999999998E-5</v>
+        <v>0.71000000000000008</v>
       </c>
       <c r="S7">
-        <v>3.4E-5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.4">
+        <v>0.48000000000000004</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C8" s="1">
-        <f>ROUND(AVERAGE(C3:C7),6)</f>
-        <v>3.0000000000000001E-6</v>
+        <f>AVERAGE(C3:C7)</f>
+        <v>0.19</v>
       </c>
       <c r="D8" s="1">
-        <f>ROUND(AVERAGE(D3:D7),6)</f>
-        <v>6.9999999999999999E-6</v>
+        <f>AVERAGE(D3:D7)</f>
+        <v>0.186</v>
       </c>
       <c r="E8" s="1">
-        <f>ROUND(AVERAGE(E3:E7),6)</f>
-        <v>1.2999999999999999E-5</v>
+        <f>AVERAGE(E3:E7)</f>
+        <v>0.18</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>1</v>
       </c>
       <c r="J8" s="1">
-        <f>ROUND(AVERAGE(J3:J7),6)</f>
-        <v>3.9999999999999998E-6</v>
+        <f>AVERAGE(J3:J7)</f>
+        <v>0.20400000000000001</v>
       </c>
       <c r="K8" s="1">
-        <f>ROUND(AVERAGE(K3:K7),6)</f>
-        <v>6.9999999999999999E-6</v>
+        <f>AVERAGE(K3:K7)</f>
+        <v>0.182</v>
       </c>
       <c r="L8" s="1">
-        <f>ROUND(AVERAGE(L3:L7),6)</f>
-        <v>1.2E-5</v>
+        <f>AVERAGE(L3:L7)</f>
+        <v>0.17600000000000002</v>
       </c>
       <c r="P8" s="1" t="s">
         <v>1</v>
       </c>
       <c r="Q8" s="1">
         <f>ROUND(AVERAGE(Q3:Q7),6)</f>
-        <v>2.3E-5</v>
+        <v>2.4860000000000002</v>
       </c>
       <c r="R8" s="1">
         <f>ROUND(AVERAGE(R3:R7),6)</f>
-        <v>2.8E-5</v>
+        <v>0.72399999999999998</v>
       </c>
       <c r="S8" s="1">
         <f>ROUND(AVERAGE(S3:S7),6)</f>
-        <v>3.1999999999999999E-5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.4">
+        <v>0.46600000000000003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
       <c r="C9">
-        <v>2.5300000000000002E-4</v>
+        <v>97.14</v>
       </c>
       <c r="D9">
-        <v>2.6499999999999999E-4</v>
+        <v>11.67</v>
       </c>
       <c r="E9">
-        <v>2.7399999999999999E-4</v>
+        <v>3.92</v>
       </c>
       <c r="H9" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="I9">
         <v>1</v>
       </c>
       <c r="J9">
-        <v>1.65E-4</v>
+        <v>91.92</v>
       </c>
       <c r="K9">
-        <v>1.7200000000000001E-4</v>
+        <v>9.89</v>
       </c>
       <c r="L9">
-        <v>1.8200000000000001E-4</v>
+        <v>3.3</v>
       </c>
       <c r="O9" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="P9">
         <v>1</v>
       </c>
       <c r="Q9">
-        <v>6.0219999999999996E-3</v>
+        <v>2017.1</v>
       </c>
       <c r="R9">
-        <v>1.3429E-2</v>
+        <v>544.87</v>
       </c>
       <c r="S9">
-        <v>2.3667000000000001E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.4">
+        <v>401.55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B10">
         <v>2</v>
       </c>
       <c r="C10">
-        <v>2.5799999999999998E-4</v>
+        <v>95.69</v>
       </c>
       <c r="D10">
-        <v>2.6200000000000003E-4</v>
+        <v>11.4</v>
       </c>
       <c r="E10">
-        <v>2.7300000000000002E-4</v>
+        <v>3.86</v>
       </c>
       <c r="H10" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="I10">
         <v>2</v>
       </c>
       <c r="J10">
-        <v>1.6799999999999999E-4</v>
+        <v>90.8</v>
       </c>
       <c r="K10">
-        <v>1.7200000000000001E-4</v>
+        <v>10.130000000000001</v>
       </c>
       <c r="L10">
-        <v>1.8699999999999999E-4</v>
+        <v>3.32</v>
       </c>
       <c r="O10" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="P10">
         <v>2</v>
       </c>
       <c r="Q10">
-        <v>5.9100000000000003E-3</v>
+        <v>2016.47</v>
       </c>
       <c r="R10">
-        <v>1.3310000000000001E-2</v>
+        <v>544.66999999999996</v>
       </c>
       <c r="S10">
-        <v>2.3626999999999999E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.4">
+        <v>401.01</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>3</v>
       </c>
       <c r="C11">
-        <v>2.61E-4</v>
+        <v>95.67</v>
       </c>
       <c r="D11">
-        <v>2.61E-4</v>
+        <v>10.97</v>
       </c>
       <c r="E11">
-        <v>2.6600000000000001E-4</v>
+        <v>4.05</v>
       </c>
       <c r="I11">
         <v>3</v>
       </c>
       <c r="J11">
-        <v>1.6799999999999999E-4</v>
+        <v>90.72</v>
       </c>
       <c r="K11">
-        <v>1.74E-4</v>
+        <v>9.5399999999999991</v>
       </c>
       <c r="L11">
-        <v>1.85E-4</v>
+        <v>3.24</v>
       </c>
       <c r="P11">
         <v>3</v>
       </c>
       <c r="Q11">
-        <v>6.28E-3</v>
+        <v>2019.06</v>
       </c>
       <c r="R11">
-        <v>1.3271E-2</v>
+        <v>544.04</v>
       </c>
       <c r="S11">
-        <v>2.3855000000000001E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.4">
+        <v>399.99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>4</v>
       </c>
       <c r="C12">
-        <v>2.7E-4</v>
+        <v>95.860000000000014</v>
       </c>
       <c r="D12">
-        <v>2.7900000000000001E-4</v>
+        <v>10.98</v>
       </c>
       <c r="E12">
-        <v>2.8200000000000002E-4</v>
+        <v>4.21</v>
       </c>
       <c r="I12">
         <v>4</v>
       </c>
       <c r="J12">
-        <v>1.6899999999999999E-4</v>
+        <v>90.75</v>
       </c>
       <c r="K12">
-        <v>1.6899999999999999E-4</v>
+        <v>9.5299999999999994</v>
       </c>
       <c r="L12">
-        <v>1.85E-4</v>
+        <v>3.6900000000000004</v>
       </c>
       <c r="P12">
         <v>4</v>
       </c>
       <c r="Q12">
-        <v>6.0920000000000002E-3</v>
+        <v>2017.55</v>
       </c>
       <c r="R12">
-        <v>1.3226E-2</v>
+        <v>544.48</v>
       </c>
       <c r="S12">
-        <v>2.4412E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.4">
+        <v>400.25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>5</v>
       </c>
       <c r="C13">
-        <v>2.4699999999999999E-4</v>
+        <v>96.45</v>
       </c>
       <c r="D13">
-        <v>2.5700000000000001E-4</v>
+        <v>10.959999999999999</v>
       </c>
       <c r="E13">
-        <v>2.8299999999999999E-4</v>
+        <v>3.79</v>
       </c>
       <c r="I13">
         <v>5</v>
       </c>
       <c r="J13">
-        <v>1.6699999999999999E-4</v>
+        <v>90.84</v>
       </c>
       <c r="K13">
-        <v>1.73E-4</v>
+        <v>9.5299999999999994</v>
       </c>
       <c r="L13">
-        <v>1.8599999999999999E-4</v>
+        <v>3.17</v>
       </c>
       <c r="P13">
         <v>5</v>
       </c>
       <c r="Q13">
-        <v>5.9690000000000003E-3</v>
+        <v>2014.78</v>
       </c>
       <c r="R13">
-        <v>1.3336000000000001E-2</v>
+        <v>544.48</v>
       </c>
       <c r="S13">
-        <v>2.4166E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.4">
+        <v>399.93</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B14" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C14" s="1">
-        <f>ROUND(AVERAGE(C9:C13),6)</f>
-        <v>2.5799999999999998E-4</v>
+        <f>AVERAGE(C9:C13)</f>
+        <v>96.162000000000006</v>
       </c>
       <c r="D14" s="1">
-        <f>ROUND(AVERAGE(D9:D13),6)</f>
-        <v>2.6499999999999999E-4</v>
+        <f>AVERAGE(D9:D13)</f>
+        <v>11.196</v>
       </c>
       <c r="E14" s="1">
-        <f>ROUND(AVERAGE(E9:E13),6)</f>
-        <v>2.7599999999999999E-4</v>
+        <f>AVERAGE(E9:E13)</f>
+        <v>3.9659999999999997</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>1</v>
       </c>
       <c r="J14" s="1">
-        <f>ROUND(AVERAGE(J9:J13),6)</f>
-        <v>1.6699999999999999E-4</v>
+        <f>AVERAGE(J9:J13)</f>
+        <v>91.006</v>
       </c>
       <c r="K14" s="1">
-        <f>ROUND(AVERAGE(K9:K13),6)</f>
-        <v>1.7200000000000001E-4</v>
+        <f>AVERAGE(K9:K13)</f>
+        <v>9.7240000000000002</v>
       </c>
       <c r="L14" s="1">
-        <f>ROUND(AVERAGE(L9:L13),6)</f>
-        <v>1.85E-4</v>
+        <f>AVERAGE(L9:L13)</f>
+        <v>3.3439999999999999</v>
       </c>
       <c r="P14" s="1" t="s">
         <v>1</v>
       </c>
       <c r="Q14" s="1">
         <f>ROUND(AVERAGE(Q9:Q13),6)</f>
-        <v>6.0549999999999996E-3</v>
+        <v>2016.992</v>
       </c>
       <c r="R14" s="1">
         <f>ROUND(AVERAGE(R9:R13),6)</f>
-        <v>1.3313999999999999E-2</v>
+        <v>544.50800000000004</v>
       </c>
       <c r="S14" s="1">
         <f>ROUND(AVERAGE(S9:S13),6)</f>
-        <v>2.3945000000000001E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.4">
+        <v>400.54599999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
       <c r="C15">
-        <v>1.7100000000000001E-4</v>
+        <v>97.649999999999991</v>
       </c>
       <c r="D15">
-        <v>1.7699999999999999E-4</v>
+        <v>11.76</v>
       </c>
       <c r="E15">
-        <v>1.83E-4</v>
+        <v>4.0200000000000005</v>
       </c>
       <c r="H15" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="I15">
         <v>1</v>
       </c>
       <c r="J15">
-        <v>1.22E-4</v>
+        <v>92.350000000000009</v>
       </c>
       <c r="K15">
-        <v>1.25E-4</v>
+        <v>9.9</v>
       </c>
       <c r="L15">
-        <v>1.34E-4</v>
+        <v>3.22</v>
       </c>
       <c r="O15" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="P15">
         <v>1</v>
       </c>
       <c r="Q15">
-        <v>8.7360000000000007E-3</v>
+        <v>2952.8700000000003</v>
       </c>
       <c r="R15">
-        <v>2.5623E-2</v>
+        <v>1051.1099999999999</v>
       </c>
       <c r="S15">
-        <v>9.1319999999999998E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.4">
+        <v>1529.1599999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B16">
         <v>2</v>
       </c>
       <c r="C16">
-        <v>1.73E-4</v>
+        <v>96.28</v>
       </c>
       <c r="D16">
-        <v>1.76E-4</v>
+        <v>11.26</v>
       </c>
       <c r="E16">
-        <v>1.8699999999999999E-4</v>
+        <v>4.03</v>
       </c>
       <c r="H16" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="I16">
         <v>2</v>
       </c>
       <c r="J16">
-        <v>1.2300000000000001E-4</v>
+        <v>90.460000000000008</v>
       </c>
       <c r="K16">
-        <v>1.25E-4</v>
+        <v>10.209999999999999</v>
       </c>
       <c r="L16">
-        <v>1.6699999999999999E-4</v>
+        <v>3.35</v>
       </c>
       <c r="O16" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="P16">
         <v>2</v>
       </c>
       <c r="Q16">
-        <v>8.5629999999999994E-3</v>
+        <v>2957.63</v>
       </c>
       <c r="R16">
-        <v>2.5531000000000002E-2</v>
+        <v>1050.7</v>
       </c>
       <c r="S16">
-        <v>9.1296000000000002E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.4">
+        <v>1527.64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B17">
         <v>3</v>
       </c>
       <c r="C17">
-        <v>1.73E-4</v>
+        <v>96.5</v>
       </c>
       <c r="D17">
-        <v>1.7699999999999999E-4</v>
+        <v>10.85</v>
       </c>
       <c r="E17">
-        <v>1.8799999999999999E-4</v>
+        <v>4.03</v>
       </c>
       <c r="I17">
         <v>3</v>
       </c>
       <c r="J17">
-        <v>1.2E-4</v>
+        <v>90.449999999999989</v>
       </c>
       <c r="K17">
-        <v>1.26E-4</v>
+        <v>9.4799999999999986</v>
       </c>
       <c r="L17">
-        <v>1.3300000000000001E-4</v>
+        <v>3.64</v>
       </c>
       <c r="P17">
         <v>3</v>
       </c>
       <c r="Q17">
-        <v>8.5939999999999992E-3</v>
+        <v>2957.25</v>
       </c>
       <c r="R17">
-        <v>2.5513000000000001E-2</v>
+        <v>1050.6699999999998</v>
       </c>
       <c r="S17">
-        <v>9.1105000000000005E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.4">
+        <v>1527.29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B18">
         <v>4</v>
       </c>
       <c r="C18">
-        <v>1.6899999999999999E-4</v>
+        <v>96.35</v>
       </c>
       <c r="D18">
-        <v>1.7799999999999999E-4</v>
+        <v>10.809999999999999</v>
       </c>
       <c r="E18">
-        <v>1.8699999999999999E-4</v>
+        <v>4.2</v>
       </c>
       <c r="I18">
         <v>4</v>
       </c>
       <c r="J18">
-        <v>1.21E-4</v>
+        <v>90.71</v>
       </c>
       <c r="K18">
-        <v>1.25E-4</v>
+        <v>9.5</v>
       </c>
       <c r="L18">
-        <v>1.35E-4</v>
+        <v>3.97</v>
       </c>
       <c r="P18">
         <v>4</v>
       </c>
       <c r="Q18">
-        <v>8.6099999999999996E-3</v>
+        <v>2955.64</v>
       </c>
       <c r="R18">
-        <v>2.5530000000000001E-2</v>
+        <v>1049.95</v>
       </c>
       <c r="S18">
-        <v>9.1203999999999993E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.4">
+        <v>1529.1399999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B19">
         <v>5</v>
       </c>
       <c r="C19">
-        <v>1.7200000000000001E-4</v>
+        <v>96.179999999999993</v>
       </c>
       <c r="D19">
-        <v>1.8000000000000001E-4</v>
+        <v>10.83</v>
       </c>
       <c r="E19">
-        <v>1.9599999999999999E-4</v>
+        <v>3.7199999999999998</v>
       </c>
       <c r="I19">
         <v>5</v>
       </c>
       <c r="J19">
-        <v>1.1900000000000001E-4</v>
+        <v>90.48</v>
       </c>
       <c r="K19">
-        <v>1.25E-4</v>
+        <v>9.4799999999999986</v>
       </c>
       <c r="L19">
-        <v>1.3300000000000001E-4</v>
+        <v>3.24</v>
       </c>
       <c r="P19">
         <v>5</v>
       </c>
       <c r="Q19">
-        <v>8.6029999999999995E-3</v>
+        <v>2956.86</v>
       </c>
       <c r="R19">
-        <v>2.5510999999999999E-2</v>
+        <v>1050</v>
       </c>
       <c r="S19">
-        <v>9.1567999999999997E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.4">
+        <v>1527.56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B20" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C20" s="1">
-        <f>ROUND(AVERAGE(C15:C19),6)</f>
-        <v>1.7200000000000001E-4</v>
+        <f>AVERAGE(C15:C19)</f>
+        <v>96.591999999999999</v>
       </c>
       <c r="D20" s="1">
-        <f>ROUND(AVERAGE(D15:D19),6)</f>
-        <v>1.7799999999999999E-4</v>
+        <f>AVERAGE(D15:D19)</f>
+        <v>11.101999999999999</v>
       </c>
       <c r="E20" s="1">
-        <f>ROUND(AVERAGE(E15:E19),6)</f>
-        <v>1.8799999999999999E-4</v>
+        <f>AVERAGE(E15:E19)</f>
+        <v>4</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>1</v>
       </c>
       <c r="J20" s="1">
-        <f>ROUND(AVERAGE(J15:J19),6)</f>
-        <v>1.21E-4</v>
+        <f>AVERAGE(J15:J19)</f>
+        <v>90.89</v>
       </c>
       <c r="K20" s="1">
-        <f>ROUND(AVERAGE(K15:K19),6)</f>
-        <v>1.25E-4</v>
+        <f>AVERAGE(K15:K19)</f>
+        <v>9.7139999999999986</v>
       </c>
       <c r="L20" s="1">
-        <f>ROUND(AVERAGE(L15:L19),6)</f>
-        <v>1.3999999999999999E-4</v>
+        <f>AVERAGE(L15:L19)</f>
+        <v>3.4840000000000004</v>
       </c>
       <c r="P20" s="1" t="s">
         <v>1</v>
       </c>
       <c r="Q20" s="1">
         <f>ROUND(AVERAGE(Q15:Q19),6)</f>
-        <v>8.6210000000000002E-3</v>
+        <v>2956.05</v>
       </c>
       <c r="R20" s="1">
         <f>ROUND(AVERAGE(R15:R19),6)</f>
-        <v>2.5541999999999999E-2</v>
+        <v>1050.4860000000001</v>
       </c>
       <c r="S20" s="1">
         <f>ROUND(AVERAGE(S15:S19),6)</f>
-        <v>9.1299000000000005E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.4">
+        <v>1528.1579999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>84.02</v>
+      </c>
+      <c r="D21">
+        <v>9.7799999999999994</v>
+      </c>
+      <c r="E21">
+        <v>3.44</v>
+      </c>
+      <c r="H21" t="s">
+        <v>8</v>
+      </c>
+      <c r="I21">
+        <v>1</v>
+      </c>
+      <c r="J21">
+        <v>76.81</v>
+      </c>
+      <c r="K21">
+        <v>8.14</v>
+      </c>
+      <c r="L21">
+        <v>2.67</v>
+      </c>
+      <c r="O21" t="s">
+        <v>9</v>
+      </c>
+      <c r="P21">
+        <v>1</v>
+      </c>
+      <c r="Q21">
+        <v>4005.92</v>
+      </c>
+      <c r="R21">
+        <v>1084.6500000000001</v>
+      </c>
+      <c r="S21">
+        <v>789.06000000000006</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>6</v>
-      </c>
-      <c r="B21">
-        <v>1</v>
-      </c>
-      <c r="C21">
-        <v>1.6899999999999999E-4</v>
-      </c>
-      <c r="D21">
-        <v>1.75E-4</v>
-      </c>
-      <c r="E21">
-        <v>1.83E-4</v>
-      </c>
-      <c r="H21" t="s">
-        <v>11</v>
-      </c>
-      <c r="I21">
-        <v>1</v>
-      </c>
-      <c r="J21">
-        <v>1.18E-4</v>
-      </c>
-      <c r="K21">
-        <v>1.2400000000000001E-4</v>
-      </c>
-      <c r="L21">
-        <v>1.3100000000000001E-4</v>
-      </c>
-      <c r="O21" t="s">
-        <v>12</v>
-      </c>
-      <c r="P21">
-        <v>1</v>
-      </c>
-      <c r="Q21">
-        <v>1.2184E-2</v>
-      </c>
-      <c r="R21">
-        <v>2.6356999999999998E-2</v>
-      </c>
-      <c r="S21">
-        <v>4.7480000000000001E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="A22" t="s">
-        <v>9</v>
       </c>
       <c r="B22">
         <v>2</v>
       </c>
       <c r="C22">
-        <v>1.73E-4</v>
+        <v>82.92</v>
       </c>
       <c r="D22">
-        <v>1.7899999999999999E-4</v>
+        <v>9.84</v>
       </c>
       <c r="E22">
-        <v>1.85E-4</v>
+        <v>3.44</v>
       </c>
       <c r="H22" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="I22">
         <v>2</v>
       </c>
       <c r="J22">
-        <v>1.21E-4</v>
+        <v>75.62</v>
       </c>
       <c r="K22">
-        <v>1.27E-4</v>
+        <v>8.49</v>
       </c>
       <c r="L22">
-        <v>1.35E-4</v>
+        <v>2.62</v>
       </c>
       <c r="O22" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="P22">
         <v>2</v>
       </c>
       <c r="Q22">
-        <v>1.2128999999999999E-2</v>
+        <v>3998.43</v>
       </c>
       <c r="R22">
-        <v>2.6199E-2</v>
+        <v>1081.43</v>
       </c>
       <c r="S22">
-        <v>4.7120000000000002E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.4">
+        <v>788.3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B23">
         <v>3</v>
       </c>
       <c r="C23">
-        <v>1.73E-4</v>
+        <v>82.93</v>
       </c>
       <c r="D23">
-        <v>1.73E-4</v>
+        <v>9.3899999999999988</v>
       </c>
       <c r="E23">
-        <v>1.8699999999999999E-4</v>
+        <v>3.61</v>
       </c>
       <c r="I23">
         <v>3</v>
       </c>
       <c r="J23">
-        <v>1.25E-4</v>
+        <v>75.64</v>
       </c>
       <c r="K23">
-        <v>1.26E-4</v>
+        <v>7.7700000000000005</v>
       </c>
       <c r="L23">
-        <v>1.3300000000000001E-4</v>
+        <v>2.54</v>
       </c>
       <c r="P23">
         <v>3</v>
       </c>
       <c r="Q23">
-        <v>1.2139E-2</v>
+        <v>3996.92</v>
       </c>
       <c r="R23">
-        <v>2.6224999999999998E-2</v>
+        <v>1081.1400000000001</v>
       </c>
       <c r="S23">
-        <v>4.7097E-2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.4">
+        <v>788.24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B24">
         <v>4</v>
       </c>
       <c r="C24">
-        <v>1.7000000000000001E-4</v>
+        <v>82.92</v>
       </c>
       <c r="D24">
-        <v>1.75E-4</v>
+        <v>9.34</v>
       </c>
       <c r="E24">
-        <v>1.8599999999999999E-4</v>
+        <v>3.5599999999999996</v>
       </c>
       <c r="I24">
         <v>4</v>
       </c>
       <c r="J24">
-        <v>1.21E-4</v>
+        <v>75.709999999999994</v>
       </c>
       <c r="K24">
-        <v>1.2400000000000001E-4</v>
+        <v>7.79</v>
       </c>
       <c r="L24">
-        <v>1.35E-4</v>
+        <v>2.5999999999999996</v>
       </c>
       <c r="P24">
         <v>4</v>
       </c>
       <c r="Q24">
-        <v>1.2154E-2</v>
+        <v>3998.53</v>
       </c>
       <c r="R24">
-        <v>2.6231999999999998E-2</v>
+        <v>1080.75</v>
       </c>
       <c r="S24">
-        <v>4.7063000000000001E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.4">
+        <v>788.11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B25">
         <v>5</v>
       </c>
       <c r="C25">
-        <v>1.7200000000000001E-4</v>
+        <v>82.86999999999999</v>
       </c>
       <c r="D25">
-        <v>1.83E-4</v>
+        <v>9.35</v>
       </c>
       <c r="E25">
-        <v>1.83E-4</v>
+        <v>3.5100000000000002</v>
       </c>
       <c r="I25">
         <v>5</v>
       </c>
       <c r="J25">
-        <v>1.2E-4</v>
+        <v>75.72</v>
       </c>
       <c r="K25">
-        <v>1.25E-4</v>
+        <v>7.78</v>
       </c>
       <c r="L25">
-        <v>1.3300000000000001E-4</v>
+        <v>3.06</v>
       </c>
       <c r="P25">
         <v>5</v>
       </c>
       <c r="Q25">
-        <v>1.2102999999999999E-2</v>
+        <v>4000.72</v>
       </c>
       <c r="R25">
-        <v>2.6217000000000001E-2</v>
+        <v>1081.22</v>
       </c>
       <c r="S25">
-        <v>4.7073999999999998E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.4">
+        <v>788.21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B26" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C26" s="1">
-        <f>ROUND(AVERAGE(C21:C25),6)</f>
-        <v>1.7100000000000001E-4</v>
+        <f>AVERAGE(C21:C25)</f>
+        <v>83.132000000000005</v>
       </c>
       <c r="D26" s="1">
-        <f>ROUND(AVERAGE(D21:D25),6)</f>
-        <v>1.7699999999999999E-4</v>
+        <f>AVERAGE(D21:D25)</f>
+        <v>9.5399999999999991</v>
       </c>
       <c r="E26" s="1">
-        <f>ROUND(AVERAGE(E21:E25),6)</f>
-        <v>1.85E-4</v>
+        <f>AVERAGE(E21:E25)</f>
+        <v>3.5120000000000005</v>
       </c>
       <c r="I26" s="1" t="s">
         <v>1</v>
       </c>
       <c r="J26" s="1">
-        <f>ROUND(AVERAGE(J21:J25),6)</f>
-        <v>1.21E-4</v>
+        <f>AVERAGE(J21:J25)</f>
+        <v>75.900000000000006</v>
       </c>
       <c r="K26" s="1">
-        <f>ROUND(AVERAGE(K21:K25),6)</f>
-        <v>1.25E-4</v>
+        <f>AVERAGE(K21:K25)</f>
+        <v>7.9940000000000015</v>
       </c>
       <c r="L26" s="1">
-        <f>ROUND(AVERAGE(L21:L25),6)</f>
-        <v>1.3300000000000001E-4</v>
+        <f>AVERAGE(L21:L25)</f>
+        <v>2.698</v>
       </c>
       <c r="P26" s="1" t="s">
         <v>1</v>
       </c>
       <c r="Q26" s="1">
         <f>ROUND(AVERAGE(Q21:Q25),6)</f>
-        <v>1.2142E-2</v>
+        <v>4000.1039999999998</v>
       </c>
       <c r="R26" s="1">
         <f>ROUND(AVERAGE(R21:R25),6)</f>
-        <v>2.6245999999999998E-2</v>
+        <v>1081.838</v>
       </c>
       <c r="S26" s="1">
         <f>ROUND(AVERAGE(S21:S25),6)</f>
-        <v>4.7167000000000001E-2</v>
+        <v>788.38400000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="M32">
+        <v>10000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2020/11/19 modify comment to doxygen form
</commit_message>
<xml_diff>
--- a/operation speed comparison.xlsx
+++ b/operation speed comparison.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\source\repos\BigIntegerGroup\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\umc19\source\repos\BigIntegerGroup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69EBEC3A-BEAF-4806-8AA2-E6693B9F2D6E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6FC71BC-72C2-4334-8C2A-A1B241A38D8A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1980" yWindow="6510" windowWidth="25065" windowHeight="11415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,21 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="18">
   <si>
     <t>add</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -92,6 +101,10 @@
   </si>
   <si>
     <t>조건: [모든 수는 non_negative, bit = 1024], [각 셀의 값은 (그 연산을 1000회 실행하는 시간의 평균값) * 10000], [mod_exp 연산에서 n = 65537] [div, mod_exp 연산시 flag = 4]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>//todo</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -451,28 +464,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S26"/>
+  <dimension ref="A1:S29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M32" sqref="M32"/>
+    <sheetView tabSelected="1" topLeftCell="B16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="2" width="9.625" customWidth="1"/>
-    <col min="3" max="5" width="14.125" customWidth="1"/>
-    <col min="8" max="9" width="9.625" customWidth="1"/>
-    <col min="10" max="12" width="14.125" customWidth="1"/>
-    <col min="15" max="16" width="9.625" customWidth="1"/>
-    <col min="17" max="19" width="14.125" customWidth="1"/>
+    <col min="1" max="2" width="9.59765625" customWidth="1"/>
+    <col min="3" max="5" width="14.09765625" customWidth="1"/>
+    <col min="8" max="9" width="9.59765625" customWidth="1"/>
+    <col min="10" max="12" width="14.09765625" customWidth="1"/>
+    <col min="15" max="16" width="9.59765625" customWidth="1"/>
+    <col min="17" max="19" width="14.09765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.4">
       <c r="C2" t="s">
         <v>13</v>
       </c>
@@ -501,7 +514,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -548,7 +561,7 @@
         <v>0.47</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.4">
       <c r="B4">
         <v>2</v>
       </c>
@@ -573,6 +586,9 @@
       <c r="L4">
         <v>0.17</v>
       </c>
+      <c r="O4" t="s">
+        <v>17</v>
+      </c>
       <c r="P4">
         <v>2</v>
       </c>
@@ -586,7 +602,7 @@
         <v>0.46</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.4">
       <c r="B5">
         <v>3</v>
       </c>
@@ -624,7 +640,7 @@
         <v>0.46</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.4">
       <c r="B6">
         <v>4</v>
       </c>
@@ -662,7 +678,7 @@
         <v>0.46</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.4">
       <c r="B7">
         <v>5</v>
       </c>
@@ -700,7 +716,7 @@
         <v>0.48000000000000004</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.4">
       <c r="B8" s="1" t="s">
         <v>1</v>
       </c>
@@ -747,7 +763,7 @@
         <v>0.46600000000000003</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -794,7 +810,7 @@
         <v>401.55</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -841,7 +857,7 @@
         <v>401.01</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.4">
       <c r="B11">
         <v>3</v>
       </c>
@@ -879,7 +895,7 @@
         <v>399.99</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.4">
       <c r="B12">
         <v>4</v>
       </c>
@@ -917,7 +933,7 @@
         <v>400.25</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.4">
       <c r="B13">
         <v>5</v>
       </c>
@@ -955,7 +971,7 @@
         <v>399.93</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.4">
       <c r="B14" s="1" t="s">
         <v>1</v>
       </c>
@@ -1002,7 +1018,7 @@
         <v>400.54599999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -1049,7 +1065,7 @@
         <v>1529.1599999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -1096,7 +1112,7 @@
         <v>1527.64</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.4">
       <c r="B17">
         <v>3</v>
       </c>
@@ -1134,7 +1150,7 @@
         <v>1527.29</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.4">
       <c r="B18">
         <v>4</v>
       </c>
@@ -1172,7 +1188,7 @@
         <v>1529.1399999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.4">
       <c r="B19">
         <v>5</v>
       </c>
@@ -1210,7 +1226,7 @@
         <v>1527.56</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.4">
       <c r="B20" s="1" t="s">
         <v>1</v>
       </c>
@@ -1257,7 +1273,7 @@
         <v>1528.1579999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>3</v>
       </c>
@@ -1304,7 +1320,7 @@
         <v>789.06000000000006</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>6</v>
       </c>
@@ -1351,7 +1367,7 @@
         <v>788.3</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.4">
       <c r="B23">
         <v>3</v>
       </c>
@@ -1389,7 +1405,7 @@
         <v>788.24</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.4">
       <c r="B24">
         <v>4</v>
       </c>
@@ -1427,7 +1443,7 @@
         <v>788.11</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.4">
       <c r="B25">
         <v>5</v>
       </c>
@@ -1465,7 +1481,7 @@
         <v>788.21</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.4">
       <c r="B26" s="1" t="s">
         <v>1</v>
       </c>
@@ -1510,6 +1526,11 @@
       <c r="S26" s="1">
         <f>ROUND(AVERAGE(S21:S25),6)</f>
         <v>788.38400000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="H29">
+        <v>0.16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2020/11/20 Update operation speed comparison
</commit_message>
<xml_diff>
--- a/operation speed comparison.xlsx
+++ b/operation speed comparison.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\umc19\source\repos\BigIntegerGroup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6FC71BC-72C2-4334-8C2A-A1B241A38D8A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FEFA966-E152-433D-9CC2-878AE7D60814}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="19">
   <si>
     <t>add</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -100,11 +100,14 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>조건: [모든 수는 non_negative, bit = 1024], [각 셀의 값은 (그 연산을 1000회 실행하는 시간의 평균값) * 10000], [mod_exp 연산에서 n = 65537] [div, mod_exp 연산시 flag = 4]</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>//todo</t>
+    <t>gen_rand</t>
+  </si>
+  <si>
+    <t>gen_rand</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>조건: [모든 수는 non_negative, bit = 1024], [각 셀의 값은 (그 연산을 1000회 실행하는 시간의 평균값) * 10000], [div, mod_exp 연산시 flag = 4], [div 연산시 a는 2048-bit]</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -464,10 +467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S29"/>
+  <dimension ref="A1:S30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q27" sqref="Q27:S27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -482,7 +485,7 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.4">
@@ -522,13 +525,13 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>0.19</v>
+        <v>0.06</v>
       </c>
       <c r="D3">
-        <v>0.19</v>
+        <v>0.06</v>
       </c>
       <c r="E3">
-        <v>0.18</v>
+        <v>0.03</v>
       </c>
       <c r="H3" t="s">
         <v>2</v>
@@ -537,13 +540,13 @@
         <v>1</v>
       </c>
       <c r="J3">
-        <v>0.19</v>
+        <v>0.11</v>
       </c>
       <c r="K3">
-        <v>0.18</v>
+        <v>0.06</v>
       </c>
       <c r="L3">
-        <v>0.18</v>
+        <v>3.9999999999999994E-2</v>
       </c>
       <c r="O3" t="s">
         <v>7</v>
@@ -552,13 +555,13 @@
         <v>1</v>
       </c>
       <c r="Q3">
-        <v>2.39</v>
+        <v>15.940000000000001</v>
       </c>
       <c r="R3">
-        <v>0.72</v>
+        <v>9.26</v>
       </c>
       <c r="S3">
-        <v>0.47</v>
+        <v>6.7</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.4">
@@ -566,40 +569,37 @@
         <v>2</v>
       </c>
       <c r="C4">
-        <v>0.19</v>
+        <v>2.0000000000000004E-2</v>
       </c>
       <c r="D4">
-        <v>0.18</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>0.18</v>
+        <v>-1.0000000000000002E-2</v>
       </c>
       <c r="I4">
         <v>2</v>
       </c>
       <c r="J4">
-        <v>0.19</v>
+        <v>9.999999999999995E-3</v>
       </c>
       <c r="K4">
-        <v>0.17</v>
+        <v>0.03</v>
       </c>
       <c r="L4">
-        <v>0.17</v>
-      </c>
-      <c r="O4" t="s">
-        <v>17</v>
+        <v>-1.0000000000000002E-2</v>
       </c>
       <c r="P4">
         <v>2</v>
       </c>
       <c r="Q4">
-        <v>2.4</v>
+        <v>17.170000000000002</v>
       </c>
       <c r="R4">
-        <v>0.74999999999999989</v>
+        <v>9.5400000000000009</v>
       </c>
       <c r="S4">
-        <v>0.46</v>
+        <v>6.5600000000000005</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.4">
@@ -607,37 +607,37 @@
         <v>3</v>
       </c>
       <c r="C5">
-        <v>0.19</v>
+        <v>9.999999999999995E-3</v>
       </c>
       <c r="D5">
-        <v>0.19</v>
+        <v>9.999999999999995E-3</v>
       </c>
       <c r="E5">
-        <v>0.18</v>
+        <v>9.999999999999995E-3</v>
       </c>
       <c r="I5">
         <v>3</v>
       </c>
       <c r="J5">
-        <v>0.2</v>
+        <v>9.999999999999995E-3</v>
       </c>
       <c r="K5">
-        <v>0.18</v>
+        <v>0.03</v>
       </c>
       <c r="L5">
-        <v>0.18</v>
+        <v>0</v>
       </c>
       <c r="P5">
         <v>3</v>
       </c>
       <c r="Q5">
-        <v>2.3699999999999997</v>
+        <v>17.350000000000001</v>
       </c>
       <c r="R5">
-        <v>0.72</v>
+        <v>14.35</v>
       </c>
       <c r="S5">
-        <v>0.46</v>
+        <v>5.73</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.4">
@@ -645,37 +645,37 @@
         <v>4</v>
       </c>
       <c r="C6">
-        <v>0.19</v>
+        <v>9.999999999999995E-3</v>
       </c>
       <c r="D6">
-        <v>0.19</v>
+        <v>0</v>
       </c>
       <c r="E6">
-        <v>0.18</v>
+        <v>2.0000000000000004E-2</v>
       </c>
       <c r="I6">
         <v>4</v>
       </c>
       <c r="J6">
-        <v>0.22</v>
+        <v>2.0000000000000004E-2</v>
       </c>
       <c r="K6">
-        <v>0.18</v>
+        <v>2.0000000000000004E-2</v>
       </c>
       <c r="L6">
-        <v>0.17</v>
+        <v>9.999999999999995E-3</v>
       </c>
       <c r="P6">
         <v>4</v>
       </c>
       <c r="Q6">
-        <v>2.5300000000000002</v>
+        <v>13.620000000000001</v>
       </c>
       <c r="R6">
-        <v>0.72</v>
+        <v>17.05</v>
       </c>
       <c r="S6">
-        <v>0.46</v>
+        <v>5.2700000000000005</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.4">
@@ -683,37 +683,37 @@
         <v>5</v>
       </c>
       <c r="C7">
-        <v>0.19</v>
+        <v>0</v>
       </c>
       <c r="D7">
-        <v>0.18</v>
+        <v>2.0000000000000004E-2</v>
       </c>
       <c r="E7">
-        <v>0.18</v>
+        <v>9.999999999999995E-3</v>
       </c>
       <c r="I7">
         <v>5</v>
       </c>
       <c r="J7">
-        <v>0.22</v>
+        <v>3.9999999999999994E-2</v>
       </c>
       <c r="K7">
-        <v>0.2</v>
+        <v>9.999999999999995E-3</v>
       </c>
       <c r="L7">
-        <v>0.18</v>
+        <v>0</v>
       </c>
       <c r="P7">
         <v>5</v>
       </c>
       <c r="Q7">
-        <v>2.7399999999999998</v>
+        <v>13.74</v>
       </c>
       <c r="R7">
-        <v>0.71000000000000008</v>
+        <v>7.49</v>
       </c>
       <c r="S7">
-        <v>0.48000000000000004</v>
+        <v>5.22</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.4">
@@ -721,46 +721,46 @@
         <v>1</v>
       </c>
       <c r="C8" s="1">
-        <f>AVERAGE(C3:C7)</f>
-        <v>0.19</v>
+        <f t="shared" ref="C8:E8" si="0">AVERAGE(C3:C7)</f>
+        <v>1.9999999999999997E-2</v>
       </c>
       <c r="D8" s="1">
-        <f>AVERAGE(D3:D7)</f>
-        <v>0.186</v>
+        <f t="shared" si="0"/>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="E8" s="1">
-        <f>AVERAGE(E3:E7)</f>
-        <v>0.18</v>
+        <f t="shared" si="0"/>
+        <v>1.1999999999999999E-2</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>1</v>
       </c>
       <c r="J8" s="1">
-        <f>AVERAGE(J3:J7)</f>
-        <v>0.20400000000000001</v>
+        <f t="shared" ref="J8:L8" si="1">AVERAGE(J3:J7)</f>
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="K8" s="1">
-        <f>AVERAGE(K3:K7)</f>
-        <v>0.182</v>
+        <f t="shared" si="1"/>
+        <v>3.0000000000000006E-2</v>
       </c>
       <c r="L8" s="1">
-        <f>AVERAGE(L3:L7)</f>
-        <v>0.17600000000000002</v>
+        <f t="shared" si="1"/>
+        <v>7.9999999999999967E-3</v>
       </c>
       <c r="P8" s="1" t="s">
         <v>1</v>
       </c>
       <c r="Q8" s="1">
-        <f>ROUND(AVERAGE(Q3:Q7),6)</f>
-        <v>2.4860000000000002</v>
+        <f t="shared" ref="Q8:S8" si="2">AVERAGE(Q3:Q7)</f>
+        <v>15.563999999999998</v>
       </c>
       <c r="R8" s="1">
-        <f>ROUND(AVERAGE(R3:R7),6)</f>
-        <v>0.72399999999999998</v>
+        <f t="shared" si="2"/>
+        <v>11.538</v>
       </c>
       <c r="S8" s="1">
-        <f>ROUND(AVERAGE(S3:S7),6)</f>
-        <v>0.46600000000000003</v>
+        <f t="shared" si="2"/>
+        <v>5.8959999999999999</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.4">
@@ -771,13 +771,13 @@
         <v>1</v>
       </c>
       <c r="C9">
-        <v>97.14</v>
+        <v>30.12</v>
       </c>
       <c r="D9">
-        <v>11.67</v>
+        <v>3.45</v>
       </c>
       <c r="E9">
-        <v>3.92</v>
+        <v>1.0899999999999999</v>
       </c>
       <c r="H9" t="s">
         <v>8</v>
@@ -786,28 +786,19 @@
         <v>1</v>
       </c>
       <c r="J9">
-        <v>91.92</v>
+        <v>27.39</v>
       </c>
       <c r="K9">
-        <v>9.89</v>
+        <v>3.18</v>
       </c>
       <c r="L9">
-        <v>3.3</v>
+        <v>0.92999999999999994</v>
       </c>
       <c r="O9" t="s">
         <v>9</v>
       </c>
       <c r="P9">
         <v>1</v>
-      </c>
-      <c r="Q9">
-        <v>2017.1</v>
-      </c>
-      <c r="R9">
-        <v>544.87</v>
-      </c>
-      <c r="S9">
-        <v>401.55</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.4">
@@ -818,13 +809,13 @@
         <v>2</v>
       </c>
       <c r="C10">
-        <v>95.69</v>
+        <v>44.67</v>
       </c>
       <c r="D10">
-        <v>11.4</v>
+        <v>3.64</v>
       </c>
       <c r="E10">
-        <v>3.86</v>
+        <v>0.80999999999999994</v>
       </c>
       <c r="H10" t="s">
         <v>4</v>
@@ -833,28 +824,19 @@
         <v>2</v>
       </c>
       <c r="J10">
-        <v>90.8</v>
+        <v>35.550000000000004</v>
       </c>
       <c r="K10">
-        <v>10.130000000000001</v>
+        <v>3.12</v>
       </c>
       <c r="L10">
-        <v>3.32</v>
+        <v>1.1099999999999999</v>
       </c>
       <c r="O10" t="s">
         <v>10</v>
       </c>
       <c r="P10">
         <v>2</v>
-      </c>
-      <c r="Q10">
-        <v>2016.47</v>
-      </c>
-      <c r="R10">
-        <v>544.66999999999996</v>
-      </c>
-      <c r="S10">
-        <v>401.01</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.4">
@@ -862,37 +844,28 @@
         <v>3</v>
       </c>
       <c r="C11">
-        <v>95.67</v>
+        <v>25.15</v>
       </c>
       <c r="D11">
-        <v>10.97</v>
+        <v>3.87</v>
       </c>
       <c r="E11">
-        <v>4.05</v>
+        <v>0.83</v>
       </c>
       <c r="I11">
         <v>3</v>
       </c>
       <c r="J11">
-        <v>90.72</v>
+        <v>26.33</v>
       </c>
       <c r="K11">
-        <v>9.5399999999999991</v>
+        <v>3.24</v>
       </c>
       <c r="L11">
-        <v>3.24</v>
+        <v>0.72</v>
       </c>
       <c r="P11">
         <v>3</v>
-      </c>
-      <c r="Q11">
-        <v>2019.06</v>
-      </c>
-      <c r="R11">
-        <v>544.04</v>
-      </c>
-      <c r="S11">
-        <v>399.99</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.4">
@@ -900,37 +873,28 @@
         <v>4</v>
       </c>
       <c r="C12">
-        <v>95.860000000000014</v>
+        <v>24.9</v>
       </c>
       <c r="D12">
-        <v>10.98</v>
+        <v>3.4400000000000004</v>
       </c>
       <c r="E12">
-        <v>4.21</v>
+        <v>1</v>
       </c>
       <c r="I12">
         <v>4</v>
       </c>
       <c r="J12">
-        <v>90.75</v>
+        <v>47.620000000000005</v>
       </c>
       <c r="K12">
-        <v>9.5299999999999994</v>
+        <v>2.97</v>
       </c>
       <c r="L12">
-        <v>3.6900000000000004</v>
+        <v>0.95</v>
       </c>
       <c r="P12">
         <v>4</v>
-      </c>
-      <c r="Q12">
-        <v>2017.55</v>
-      </c>
-      <c r="R12">
-        <v>544.48</v>
-      </c>
-      <c r="S12">
-        <v>400.25</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.4">
@@ -938,85 +902,67 @@
         <v>5</v>
       </c>
       <c r="C13">
-        <v>96.45</v>
+        <v>25.66</v>
       </c>
       <c r="D13">
-        <v>10.959999999999999</v>
+        <v>3.12</v>
       </c>
       <c r="E13">
-        <v>3.79</v>
+        <v>0.90999999999999992</v>
       </c>
       <c r="I13">
         <v>5</v>
       </c>
       <c r="J13">
-        <v>90.84</v>
+        <v>28.38</v>
       </c>
       <c r="K13">
-        <v>9.5299999999999994</v>
+        <v>3.06</v>
       </c>
       <c r="L13">
-        <v>3.17</v>
+        <v>0.92999999999999994</v>
       </c>
       <c r="P13">
         <v>5</v>
       </c>
-      <c r="Q13">
-        <v>2014.78</v>
-      </c>
-      <c r="R13">
-        <v>544.48</v>
-      </c>
-      <c r="S13">
-        <v>399.93</v>
-      </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.4">
       <c r="B14" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C14" s="1">
-        <f>AVERAGE(C9:C13)</f>
-        <v>96.162000000000006</v>
+        <f t="shared" ref="C14:E14" si="3">AVERAGE(C9:C13)</f>
+        <v>30.1</v>
       </c>
       <c r="D14" s="1">
-        <f>AVERAGE(D9:D13)</f>
-        <v>11.196</v>
+        <f t="shared" si="3"/>
+        <v>3.5040000000000004</v>
       </c>
       <c r="E14" s="1">
-        <f>AVERAGE(E9:E13)</f>
-        <v>3.9659999999999997</v>
+        <f t="shared" si="3"/>
+        <v>0.92799999999999994</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>1</v>
       </c>
       <c r="J14" s="1">
-        <f>AVERAGE(J9:J13)</f>
-        <v>91.006</v>
+        <f t="shared" ref="J14" si="4">AVERAGE(J9:J13)</f>
+        <v>33.054000000000002</v>
       </c>
       <c r="K14" s="1">
-        <f>AVERAGE(K9:K13)</f>
-        <v>9.7240000000000002</v>
+        <f t="shared" ref="K14" si="5">AVERAGE(K9:K13)</f>
+        <v>3.1140000000000003</v>
       </c>
       <c r="L14" s="1">
-        <f>AVERAGE(L9:L13)</f>
-        <v>3.3439999999999999</v>
+        <f t="shared" ref="L14" si="6">AVERAGE(L9:L13)</f>
+        <v>0.92799999999999994</v>
       </c>
       <c r="P14" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="Q14" s="1">
-        <f>ROUND(AVERAGE(Q9:Q13),6)</f>
-        <v>2016.992</v>
-      </c>
-      <c r="R14" s="1">
-        <f>ROUND(AVERAGE(R9:R13),6)</f>
-        <v>544.50800000000004</v>
-      </c>
-      <c r="S14" s="1">
-        <f>ROUND(AVERAGE(S9:S13),6)</f>
-        <v>400.54599999999999</v>
-      </c>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="1"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
@@ -1026,13 +972,13 @@
         <v>1</v>
       </c>
       <c r="C15">
-        <v>97.649999999999991</v>
+        <v>28.88</v>
       </c>
       <c r="D15">
-        <v>11.76</v>
+        <v>3.8600000000000003</v>
       </c>
       <c r="E15">
-        <v>4.0200000000000005</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="H15" t="s">
         <v>8</v>
@@ -1041,28 +987,19 @@
         <v>1</v>
       </c>
       <c r="J15">
-        <v>92.350000000000009</v>
+        <v>28.02</v>
       </c>
       <c r="K15">
-        <v>9.9</v>
+        <v>3.47</v>
       </c>
       <c r="L15">
-        <v>3.22</v>
+        <v>0.85</v>
       </c>
       <c r="O15" t="s">
         <v>9</v>
       </c>
       <c r="P15">
         <v>1</v>
-      </c>
-      <c r="Q15">
-        <v>2952.8700000000003</v>
-      </c>
-      <c r="R15">
-        <v>1051.1099999999999</v>
-      </c>
-      <c r="S15">
-        <v>1529.1599999999999</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.4">
@@ -1073,13 +1010,13 @@
         <v>2</v>
       </c>
       <c r="C16">
-        <v>96.28</v>
+        <v>37.230000000000004</v>
       </c>
       <c r="D16">
-        <v>11.26</v>
+        <v>3.37</v>
       </c>
       <c r="E16">
-        <v>4.03</v>
+        <v>0.82</v>
       </c>
       <c r="H16" t="s">
         <v>5</v>
@@ -1088,28 +1025,19 @@
         <v>2</v>
       </c>
       <c r="J16">
-        <v>90.460000000000008</v>
+        <v>24.89</v>
       </c>
       <c r="K16">
-        <v>10.209999999999999</v>
+        <v>3.47</v>
       </c>
       <c r="L16">
-        <v>3.35</v>
+        <v>0.87</v>
       </c>
       <c r="O16" t="s">
         <v>11</v>
       </c>
       <c r="P16">
         <v>2</v>
-      </c>
-      <c r="Q16">
-        <v>2957.63</v>
-      </c>
-      <c r="R16">
-        <v>1050.7</v>
-      </c>
-      <c r="S16">
-        <v>1527.64</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.4">
@@ -1117,37 +1045,28 @@
         <v>3</v>
       </c>
       <c r="C17">
-        <v>96.5</v>
+        <v>26.22</v>
       </c>
       <c r="D17">
-        <v>10.85</v>
+        <v>3.81</v>
       </c>
       <c r="E17">
-        <v>4.03</v>
+        <v>1.02</v>
       </c>
       <c r="I17">
         <v>3</v>
       </c>
       <c r="J17">
-        <v>90.449999999999989</v>
+        <v>24.25</v>
       </c>
       <c r="K17">
-        <v>9.4799999999999986</v>
+        <v>2.77</v>
       </c>
       <c r="L17">
-        <v>3.64</v>
+        <v>0.75</v>
       </c>
       <c r="P17">
         <v>3</v>
-      </c>
-      <c r="Q17">
-        <v>2957.25</v>
-      </c>
-      <c r="R17">
-        <v>1050.6699999999998</v>
-      </c>
-      <c r="S17">
-        <v>1527.29</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.4">
@@ -1155,37 +1074,28 @@
         <v>4</v>
       </c>
       <c r="C18">
-        <v>96.35</v>
+        <v>25.62</v>
       </c>
       <c r="D18">
-        <v>10.809999999999999</v>
+        <v>3.5900000000000003</v>
       </c>
       <c r="E18">
-        <v>4.2</v>
+        <v>0.98</v>
       </c>
       <c r="I18">
         <v>4</v>
       </c>
       <c r="J18">
-        <v>90.71</v>
+        <v>24.52</v>
       </c>
       <c r="K18">
-        <v>9.5</v>
+        <v>3.0700000000000003</v>
       </c>
       <c r="L18">
-        <v>3.97</v>
+        <v>0.67999999999999994</v>
       </c>
       <c r="P18">
         <v>4</v>
-      </c>
-      <c r="Q18">
-        <v>2955.64</v>
-      </c>
-      <c r="R18">
-        <v>1049.95</v>
-      </c>
-      <c r="S18">
-        <v>1529.1399999999999</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.4">
@@ -1193,85 +1103,67 @@
         <v>5</v>
       </c>
       <c r="C19">
-        <v>96.179999999999993</v>
+        <v>26.34</v>
       </c>
       <c r="D19">
-        <v>10.83</v>
+        <v>3.4200000000000004</v>
       </c>
       <c r="E19">
-        <v>3.7199999999999998</v>
+        <v>1</v>
       </c>
       <c r="I19">
         <v>5</v>
       </c>
       <c r="J19">
-        <v>90.48</v>
+        <v>24.4</v>
       </c>
       <c r="K19">
-        <v>9.4799999999999986</v>
+        <v>2.85</v>
       </c>
       <c r="L19">
-        <v>3.24</v>
+        <v>0.85</v>
       </c>
       <c r="P19">
         <v>5</v>
       </c>
-      <c r="Q19">
-        <v>2956.86</v>
-      </c>
-      <c r="R19">
-        <v>1050</v>
-      </c>
-      <c r="S19">
-        <v>1527.56</v>
-      </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.4">
       <c r="B20" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C20" s="1">
-        <f>AVERAGE(C15:C19)</f>
-        <v>96.591999999999999</v>
+        <f t="shared" ref="C20" si="7">AVERAGE(C15:C19)</f>
+        <v>28.857999999999997</v>
       </c>
       <c r="D20" s="1">
-        <f>AVERAGE(D15:D19)</f>
-        <v>11.101999999999999</v>
+        <f t="shared" ref="D20" si="8">AVERAGE(D15:D19)</f>
+        <v>3.6100000000000003</v>
       </c>
       <c r="E20" s="1">
-        <f>AVERAGE(E15:E19)</f>
-        <v>4</v>
+        <f t="shared" ref="E20" si="9">AVERAGE(E15:E19)</f>
+        <v>0.99199999999999999</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>1</v>
       </c>
       <c r="J20" s="1">
-        <f>AVERAGE(J15:J19)</f>
-        <v>90.89</v>
+        <f t="shared" ref="J20" si="10">AVERAGE(J15:J19)</f>
+        <v>25.215999999999998</v>
       </c>
       <c r="K20" s="1">
-        <f>AVERAGE(K15:K19)</f>
-        <v>9.7139999999999986</v>
+        <f t="shared" ref="K20" si="11">AVERAGE(K15:K19)</f>
+        <v>3.1260000000000003</v>
       </c>
       <c r="L20" s="1">
-        <f>AVERAGE(L15:L19)</f>
-        <v>3.4840000000000004</v>
+        <f t="shared" ref="L20" si="12">AVERAGE(L15:L19)</f>
+        <v>0.79999999999999993</v>
       </c>
       <c r="P20" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="Q20" s="1">
-        <f>ROUND(AVERAGE(Q15:Q19),6)</f>
-        <v>2956.05</v>
-      </c>
-      <c r="R20" s="1">
-        <f>ROUND(AVERAGE(R15:R19),6)</f>
-        <v>1050.4860000000001</v>
-      </c>
-      <c r="S20" s="1">
-        <f>ROUND(AVERAGE(S15:S19),6)</f>
-        <v>1528.1579999999999</v>
-      </c>
+      <c r="Q20" s="1"/>
+      <c r="R20" s="1"/>
+      <c r="S20" s="1"/>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
@@ -1281,13 +1173,13 @@
         <v>1</v>
       </c>
       <c r="C21">
-        <v>84.02</v>
+        <v>27.18</v>
       </c>
       <c r="D21">
-        <v>9.7799999999999994</v>
+        <v>2.95</v>
       </c>
       <c r="E21">
-        <v>3.44</v>
+        <v>1.0799999999999998</v>
       </c>
       <c r="H21" t="s">
         <v>8</v>
@@ -1296,28 +1188,19 @@
         <v>1</v>
       </c>
       <c r="J21">
-        <v>76.81</v>
+        <v>25.7</v>
       </c>
       <c r="K21">
-        <v>8.14</v>
+        <v>2.8200000000000003</v>
       </c>
       <c r="L21">
-        <v>2.67</v>
+        <v>0.74</v>
       </c>
       <c r="O21" t="s">
         <v>9</v>
       </c>
       <c r="P21">
         <v>1</v>
-      </c>
-      <c r="Q21">
-        <v>4005.92</v>
-      </c>
-      <c r="R21">
-        <v>1084.6500000000001</v>
-      </c>
-      <c r="S21">
-        <v>789.06000000000006</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.4">
@@ -1328,13 +1211,13 @@
         <v>2</v>
       </c>
       <c r="C22">
-        <v>82.92</v>
+        <v>23.49</v>
       </c>
       <c r="D22">
-        <v>9.84</v>
+        <v>3.02</v>
       </c>
       <c r="E22">
-        <v>3.44</v>
+        <v>0.94</v>
       </c>
       <c r="H22" t="s">
         <v>6</v>
@@ -1343,28 +1226,19 @@
         <v>2</v>
       </c>
       <c r="J22">
-        <v>75.62</v>
+        <v>23.349999999999998</v>
       </c>
       <c r="K22">
-        <v>8.49</v>
+        <v>2.48</v>
       </c>
       <c r="L22">
-        <v>2.62</v>
+        <v>0.67999999999999994</v>
       </c>
       <c r="O22" t="s">
         <v>12</v>
       </c>
       <c r="P22">
         <v>2</v>
-      </c>
-      <c r="Q22">
-        <v>3998.43</v>
-      </c>
-      <c r="R22">
-        <v>1081.43</v>
-      </c>
-      <c r="S22">
-        <v>788.3</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.4">
@@ -1372,37 +1246,28 @@
         <v>3</v>
       </c>
       <c r="C23">
-        <v>82.93</v>
+        <v>23.48</v>
       </c>
       <c r="D23">
-        <v>9.3899999999999988</v>
+        <v>2.8400000000000003</v>
       </c>
       <c r="E23">
-        <v>3.61</v>
+        <v>1.03</v>
       </c>
       <c r="I23">
         <v>3</v>
       </c>
       <c r="J23">
-        <v>75.64</v>
+        <v>21.65</v>
       </c>
       <c r="K23">
-        <v>7.7700000000000005</v>
+        <v>2.6900000000000004</v>
       </c>
       <c r="L23">
-        <v>2.54</v>
+        <v>0.74</v>
       </c>
       <c r="P23">
         <v>3</v>
-      </c>
-      <c r="Q23">
-        <v>3996.92</v>
-      </c>
-      <c r="R23">
-        <v>1081.1400000000001</v>
-      </c>
-      <c r="S23">
-        <v>788.24</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.4">
@@ -1410,37 +1275,28 @@
         <v>4</v>
       </c>
       <c r="C24">
-        <v>82.92</v>
+        <v>23.23</v>
       </c>
       <c r="D24">
-        <v>9.34</v>
+        <v>3.46</v>
       </c>
       <c r="E24">
-        <v>3.5599999999999996</v>
+        <v>0.97</v>
       </c>
       <c r="I24">
         <v>4</v>
       </c>
       <c r="J24">
-        <v>75.709999999999994</v>
+        <v>21.669999999999998</v>
       </c>
       <c r="K24">
-        <v>7.79</v>
+        <v>2.6500000000000004</v>
       </c>
       <c r="L24">
-        <v>2.5999999999999996</v>
+        <v>0.83</v>
       </c>
       <c r="P24">
         <v>4</v>
-      </c>
-      <c r="Q24">
-        <v>3998.53</v>
-      </c>
-      <c r="R24">
-        <v>1080.75</v>
-      </c>
-      <c r="S24">
-        <v>788.11</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.4">
@@ -1448,89 +1304,131 @@
         <v>5</v>
       </c>
       <c r="C25">
-        <v>82.86999999999999</v>
+        <v>23.4</v>
       </c>
       <c r="D25">
-        <v>9.35</v>
+        <v>2.6900000000000004</v>
       </c>
       <c r="E25">
-        <v>3.5100000000000002</v>
+        <v>0.83</v>
       </c>
       <c r="I25">
         <v>5</v>
       </c>
       <c r="J25">
-        <v>75.72</v>
+        <v>21.47</v>
       </c>
       <c r="K25">
-        <v>7.78</v>
+        <v>2.7</v>
       </c>
       <c r="L25">
-        <v>3.06</v>
+        <v>0.72</v>
       </c>
       <c r="P25">
         <v>5</v>
       </c>
-      <c r="Q25">
-        <v>4000.72</v>
-      </c>
-      <c r="R25">
-        <v>1081.22</v>
-      </c>
-      <c r="S25">
-        <v>788.21</v>
-      </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.4">
       <c r="B26" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C26" s="1">
-        <f>AVERAGE(C21:C25)</f>
-        <v>83.132000000000005</v>
+        <f t="shared" ref="C26" si="13">AVERAGE(C21:C25)</f>
+        <v>24.155999999999999</v>
       </c>
       <c r="D26" s="1">
-        <f>AVERAGE(D21:D25)</f>
-        <v>9.5399999999999991</v>
+        <f t="shared" ref="D26" si="14">AVERAGE(D21:D25)</f>
+        <v>2.992</v>
       </c>
       <c r="E26" s="1">
-        <f>AVERAGE(E21:E25)</f>
-        <v>3.5120000000000005</v>
+        <f t="shared" ref="E26" si="15">AVERAGE(E21:E25)</f>
+        <v>0.97</v>
       </c>
       <c r="I26" s="1" t="s">
         <v>1</v>
       </c>
       <c r="J26" s="1">
-        <f>AVERAGE(J21:J25)</f>
-        <v>75.900000000000006</v>
+        <f t="shared" ref="J26" si="16">AVERAGE(J21:J25)</f>
+        <v>22.767999999999997</v>
       </c>
       <c r="K26" s="1">
-        <f>AVERAGE(K21:K25)</f>
-        <v>7.9940000000000015</v>
+        <f t="shared" ref="K26" si="17">AVERAGE(K21:K25)</f>
+        <v>2.6680000000000001</v>
       </c>
       <c r="L26" s="1">
-        <f>AVERAGE(L21:L25)</f>
-        <v>2.698</v>
+        <f t="shared" ref="L26" si="18">AVERAGE(L21:L25)</f>
+        <v>0.74199999999999999</v>
       </c>
       <c r="P26" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="Q26" s="1">
-        <f>ROUND(AVERAGE(Q21:Q25),6)</f>
-        <v>4000.1039999999998</v>
-      </c>
-      <c r="R26" s="1">
-        <f>ROUND(AVERAGE(R21:R25),6)</f>
-        <v>1081.838</v>
-      </c>
-      <c r="S26" s="1">
-        <f>ROUND(AVERAGE(S21:S25),6)</f>
-        <v>788.38400000000001</v>
+      <c r="Q26" s="1"/>
+      <c r="R26" s="1"/>
+      <c r="S26" s="1"/>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A27" t="s">
+        <v>16</v>
+      </c>
+      <c r="C27">
+        <v>0.05</v>
+      </c>
+      <c r="D27">
+        <v>0.05</v>
+      </c>
+      <c r="E27">
+        <v>0.05</v>
+      </c>
+      <c r="H27" t="s">
+        <v>17</v>
+      </c>
+      <c r="J27">
+        <v>0.09</v>
+      </c>
+      <c r="K27">
+        <v>0.09</v>
+      </c>
+      <c r="L27">
+        <v>0.09</v>
+      </c>
+      <c r="O27" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q27">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="R27">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="S27">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A28">
+        <v>1024</v>
+      </c>
+      <c r="H28">
+        <v>2048</v>
+      </c>
+      <c r="O28">
+        <v>1024</v>
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A29">
+        <v>1024</v>
+      </c>
       <c r="H29">
-        <v>0.16</v>
+        <v>1024</v>
+      </c>
+      <c r="O29">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="O30">
+        <v>1024</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2020/11/30 Create config.h file & simplify function need to optimize multiplication function
</commit_message>
<xml_diff>
--- a/operation speed comparison.xlsx
+++ b/operation speed comparison.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\umc19\source\repos\BigIntegerGroup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FEFA966-E152-433D-9CC2-878AE7D60814}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A343E20-85A4-45DF-A03D-FD249E8CE853}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -469,8 +469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q27" sqref="Q27:S27"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q9" sqref="Q9:Q26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -961,8 +961,12 @@
         <v>1</v>
       </c>
       <c r="Q14" s="1"/>
-      <c r="R14" s="1"/>
-      <c r="S14" s="1"/>
+      <c r="R14" s="1">
+        <v>15546.12012</v>
+      </c>
+      <c r="S14" s="1">
+        <v>10017.89941</v>
+      </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
@@ -1162,8 +1166,12 @@
         <v>1</v>
       </c>
       <c r="Q20" s="1"/>
-      <c r="R20" s="1"/>
-      <c r="S20" s="1"/>
+      <c r="R20" s="1">
+        <v>15355.68945</v>
+      </c>
+      <c r="S20" s="1">
+        <v>9420.85059</v>
+      </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
@@ -1363,8 +1371,12 @@
         <v>1</v>
       </c>
       <c r="Q26" s="1"/>
-      <c r="R26" s="1"/>
-      <c r="S26" s="1"/>
+      <c r="R26" s="1">
+        <v>20531.101559999999</v>
+      </c>
+      <c r="S26" s="1">
+        <v>12246.559569999999</v>
+      </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A27" t="s">

</xml_diff>